<commit_message>
Solving troubles with the select
</commit_message>
<xml_diff>
--- a/Automation/AttachedFiles/Test.xlsx
+++ b/Automation/AttachedFiles/Test.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13844E37-2728-467C-ADA4-9DC9C6C6E584}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Brand</t>
   </si>
@@ -25,19 +27,28 @@
     <t>puma</t>
   </si>
   <si>
-    <t>newbalance</t>
-  </si>
-  <si>
-    <t>reebok</t>
-  </si>
-  <si>
-    <t>nike</t>
+    <t>Order by</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Announcement</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Higher</t>
+  </si>
+  <si>
+    <t>nearDistance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -178,6 +189,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -213,6 +241,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -388,63 +433,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3">
-        <v>10.5</v>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C17FAB94-2E90-48A1-BECC-D1CC48BA2B33}">
+          <x14:formula1>
+            <xm:f>Hoja2!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C483319-4B8D-4F24-ACD3-861110F67E03}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>